<commit_message>
do func export excl: nhaphang , nhanoibo
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Teamplate_PhieuNhapHang.xlsx
+++ b/banhang24/Template/ExportExcel/Teamplate_PhieuNhapHang.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Ghi chú</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Tổng chiết khấu</t>
+  </si>
+  <si>
+    <t>Mã đặt hàng</t>
   </si>
 </sst>
 </file>
@@ -228,7 +231,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -317,7 +320,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -624,7 +630,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V29"/>
+  <dimension ref="A1:W29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -634,28 +640,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="23.42578125" style="22" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" style="22" customWidth="1"/>
-    <col min="11" max="12" width="19.7109375" style="22" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="18.140625" style="22" customWidth="1"/>
-    <col min="19" max="19" width="21.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.7109375" style="22" customWidth="1"/>
-    <col min="21" max="21" width="21.7109375" style="11" customWidth="1"/>
-    <col min="22" max="22" width="17.85546875" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="23.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" style="22" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" style="22" customWidth="1"/>
+    <col min="12" max="13" width="19.7109375" style="22" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="18.140625" style="22" customWidth="1"/>
+    <col min="20" max="20" width="21.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.7109375" style="22" customWidth="1"/>
+    <col min="22" max="22" width="21.7109375" style="11" customWidth="1"/>
+    <col min="23" max="23" width="17.85546875" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
         <v>3</v>
       </c>
@@ -677,90 +683,94 @@
       <c r="Q1" s="30"/>
       <c r="R1" s="30"/>
       <c r="S1" s="30"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="5"/>
-    </row>
-    <row r="4" spans="1:22" s="7" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T1" s="30"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="5"/>
+    </row>
+    <row r="4" spans="1:23" s="7" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="D4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="20" t="s">
+      <c r="J4" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="K4" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="L4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="M4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="20" t="s">
+      <c r="N4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="20" t="s">
+      <c r="O4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="20" t="s">
+      <c r="P4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="20" t="s">
+      <c r="Q4" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="Q4" s="20" t="s">
+      <c r="R4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="R4" s="20" t="s">
+      <c r="S4" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="S4" s="20" t="s">
+      <c r="T4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="T4" s="20" t="s">
+      <c r="U4" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="U4" s="4" t="s">
+      <c r="V4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="V4" s="9" t="s">
+      <c r="W4" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
-      <c r="B5" s="16"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="16"/>
-      <c r="D5" s="10"/>
+      <c r="D5" s="16"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="31"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="17"/>
       <c r="J5" s="31"/>
-      <c r="K5" s="21"/>
+      <c r="K5" s="31"/>
       <c r="L5" s="21"/>
       <c r="M5" s="21"/>
       <c r="N5" s="21"/>
@@ -770,21 +780,22 @@
       <c r="R5" s="21"/>
       <c r="S5" s="21"/>
       <c r="T5" s="21"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="18"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U5" s="21"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="18"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="16"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="16"/>
-      <c r="D6" s="10"/>
+      <c r="D6" s="16"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="31"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="17"/>
       <c r="J6" s="31"/>
-      <c r="K6" s="21"/>
+      <c r="K6" s="31"/>
       <c r="L6" s="21"/>
       <c r="M6" s="21"/>
       <c r="N6" s="21"/>
@@ -794,21 +805,22 @@
       <c r="R6" s="21"/>
       <c r="S6" s="21"/>
       <c r="T6" s="21"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="18"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U6" s="21"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="18"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="16"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="16"/>
-      <c r="D7" s="10"/>
+      <c r="D7" s="16"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="31"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="17"/>
       <c r="J7" s="31"/>
-      <c r="K7" s="21"/>
+      <c r="K7" s="31"/>
       <c r="L7" s="21"/>
       <c r="M7" s="21"/>
       <c r="N7" s="21"/>
@@ -818,21 +830,22 @@
       <c r="R7" s="21"/>
       <c r="S7" s="21"/>
       <c r="T7" s="21"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="18"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U7" s="21"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="18"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="16"/>
+      <c r="B8" s="2"/>
       <c r="C8" s="16"/>
-      <c r="D8" s="10"/>
+      <c r="D8" s="16"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="31"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="17"/>
       <c r="J8" s="31"/>
-      <c r="K8" s="21"/>
+      <c r="K8" s="31"/>
       <c r="L8" s="21"/>
       <c r="M8" s="21"/>
       <c r="N8" s="21"/>
@@ -842,21 +855,22 @@
       <c r="R8" s="21"/>
       <c r="S8" s="21"/>
       <c r="T8" s="21"/>
-      <c r="U8" s="12"/>
-      <c r="V8" s="18"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U8" s="21"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="18"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="16"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="16"/>
-      <c r="D9" s="10"/>
+      <c r="D9" s="16"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="31"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="17"/>
       <c r="J9" s="31"/>
-      <c r="K9" s="21"/>
+      <c r="K9" s="31"/>
       <c r="L9" s="21"/>
       <c r="M9" s="21"/>
       <c r="N9" s="21"/>
@@ -866,21 +880,22 @@
       <c r="R9" s="21"/>
       <c r="S9" s="21"/>
       <c r="T9" s="21"/>
-      <c r="U9" s="12"/>
-      <c r="V9" s="18"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U9" s="21"/>
+      <c r="V9" s="12"/>
+      <c r="W9" s="18"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="16"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="16"/>
-      <c r="D10" s="10"/>
+      <c r="D10" s="16"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="31"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="17"/>
       <c r="J10" s="31"/>
-      <c r="K10" s="21"/>
+      <c r="K10" s="31"/>
       <c r="L10" s="21"/>
       <c r="M10" s="21"/>
       <c r="N10" s="21"/>
@@ -890,21 +905,22 @@
       <c r="R10" s="21"/>
       <c r="S10" s="21"/>
       <c r="T10" s="21"/>
-      <c r="U10" s="12"/>
-      <c r="V10" s="18"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U10" s="21"/>
+      <c r="V10" s="12"/>
+      <c r="W10" s="18"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="16"/>
+      <c r="B11" s="2"/>
       <c r="C11" s="16"/>
-      <c r="D11" s="10"/>
+      <c r="D11" s="16"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="31"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="17"/>
       <c r="J11" s="31"/>
-      <c r="K11" s="21"/>
+      <c r="K11" s="31"/>
       <c r="L11" s="21"/>
       <c r="M11" s="21"/>
       <c r="N11" s="21"/>
@@ -914,21 +930,22 @@
       <c r="R11" s="21"/>
       <c r="S11" s="21"/>
       <c r="T11" s="21"/>
-      <c r="U11" s="12"/>
-      <c r="V11" s="18"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U11" s="21"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="18"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
-      <c r="B12" s="16"/>
+      <c r="B12" s="2"/>
       <c r="C12" s="16"/>
-      <c r="D12" s="10"/>
+      <c r="D12" s="16"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="31"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="17"/>
       <c r="J12" s="31"/>
-      <c r="K12" s="21"/>
+      <c r="K12" s="31"/>
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
       <c r="N12" s="21"/>
@@ -938,21 +955,22 @@
       <c r="R12" s="21"/>
       <c r="S12" s="21"/>
       <c r="T12" s="21"/>
-      <c r="U12" s="12"/>
-      <c r="V12" s="18"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U12" s="21"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="18"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="16"/>
+      <c r="B13" s="2"/>
       <c r="C13" s="16"/>
-      <c r="D13" s="10"/>
+      <c r="D13" s="16"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="31"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="17"/>
       <c r="J13" s="31"/>
-      <c r="K13" s="21"/>
+      <c r="K13" s="31"/>
       <c r="L13" s="21"/>
       <c r="M13" s="21"/>
       <c r="N13" s="21"/>
@@ -962,21 +980,22 @@
       <c r="R13" s="21"/>
       <c r="S13" s="21"/>
       <c r="T13" s="21"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="18"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U13" s="21"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="18"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="16"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="16"/>
-      <c r="D14" s="10"/>
+      <c r="D14" s="16"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="31"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="17"/>
       <c r="J14" s="31"/>
-      <c r="K14" s="21"/>
+      <c r="K14" s="31"/>
       <c r="L14" s="21"/>
       <c r="M14" s="21"/>
       <c r="N14" s="21"/>
@@ -986,21 +1005,22 @@
       <c r="R14" s="21"/>
       <c r="S14" s="21"/>
       <c r="T14" s="21"/>
-      <c r="U14" s="12"/>
-      <c r="V14" s="18"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U14" s="21"/>
+      <c r="V14" s="12"/>
+      <c r="W14" s="18"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="16"/>
+      <c r="B15" s="2"/>
       <c r="C15" s="16"/>
-      <c r="D15" s="10"/>
+      <c r="D15" s="16"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="31"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="17"/>
       <c r="J15" s="31"/>
-      <c r="K15" s="21"/>
+      <c r="K15" s="31"/>
       <c r="L15" s="21"/>
       <c r="M15" s="21"/>
       <c r="N15" s="21"/>
@@ -1010,21 +1030,22 @@
       <c r="R15" s="21"/>
       <c r="S15" s="21"/>
       <c r="T15" s="21"/>
-      <c r="U15" s="12"/>
-      <c r="V15" s="18"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U15" s="21"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="18"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="16"/>
+      <c r="B16" s="2"/>
       <c r="C16" s="16"/>
-      <c r="D16" s="10"/>
+      <c r="D16" s="16"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="31"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="17"/>
       <c r="J16" s="31"/>
-      <c r="K16" s="21"/>
+      <c r="K16" s="31"/>
       <c r="L16" s="21"/>
       <c r="M16" s="21"/>
       <c r="N16" s="21"/>
@@ -1034,21 +1055,22 @@
       <c r="R16" s="21"/>
       <c r="S16" s="21"/>
       <c r="T16" s="21"/>
-      <c r="U16" s="12"/>
-      <c r="V16" s="18"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U16" s="21"/>
+      <c r="V16" s="12"/>
+      <c r="W16" s="18"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="16"/>
+      <c r="B17" s="2"/>
       <c r="C17" s="16"/>
-      <c r="D17" s="10"/>
+      <c r="D17" s="16"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="31"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="17"/>
       <c r="J17" s="31"/>
-      <c r="K17" s="21"/>
+      <c r="K17" s="31"/>
       <c r="L17" s="21"/>
       <c r="M17" s="21"/>
       <c r="N17" s="21"/>
@@ -1058,21 +1080,22 @@
       <c r="R17" s="21"/>
       <c r="S17" s="21"/>
       <c r="T17" s="21"/>
-      <c r="U17" s="12"/>
-      <c r="V17" s="18"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U17" s="21"/>
+      <c r="V17" s="12"/>
+      <c r="W17" s="18"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="16"/>
+      <c r="B18" s="2"/>
       <c r="C18" s="16"/>
-      <c r="D18" s="10"/>
+      <c r="D18" s="16"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="31"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="17"/>
       <c r="J18" s="31"/>
-      <c r="K18" s="21"/>
+      <c r="K18" s="31"/>
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
       <c r="N18" s="21"/>
@@ -1082,21 +1105,22 @@
       <c r="R18" s="21"/>
       <c r="S18" s="21"/>
       <c r="T18" s="21"/>
-      <c r="U18" s="12"/>
-      <c r="V18" s="18"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U18" s="21"/>
+      <c r="V18" s="12"/>
+      <c r="W18" s="18"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="16"/>
+      <c r="B19" s="2"/>
       <c r="C19" s="16"/>
-      <c r="D19" s="10"/>
+      <c r="D19" s="16"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="31"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="17"/>
       <c r="J19" s="31"/>
-      <c r="K19" s="21"/>
+      <c r="K19" s="31"/>
       <c r="L19" s="21"/>
       <c r="M19" s="21"/>
       <c r="N19" s="21"/>
@@ -1106,21 +1130,22 @@
       <c r="R19" s="21"/>
       <c r="S19" s="21"/>
       <c r="T19" s="21"/>
-      <c r="U19" s="12"/>
-      <c r="V19" s="18"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U19" s="21"/>
+      <c r="V19" s="12"/>
+      <c r="W19" s="18"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="16"/>
+      <c r="B20" s="2"/>
       <c r="C20" s="16"/>
-      <c r="D20" s="10"/>
+      <c r="D20" s="16"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="31"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="17"/>
       <c r="J20" s="31"/>
-      <c r="K20" s="21"/>
+      <c r="K20" s="31"/>
       <c r="L20" s="21"/>
       <c r="M20" s="21"/>
       <c r="N20" s="21"/>
@@ -1130,21 +1155,22 @@
       <c r="R20" s="21"/>
       <c r="S20" s="21"/>
       <c r="T20" s="21"/>
-      <c r="U20" s="12"/>
-      <c r="V20" s="18"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U20" s="21"/>
+      <c r="V20" s="12"/>
+      <c r="W20" s="18"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="16"/>
+      <c r="B21" s="2"/>
       <c r="C21" s="16"/>
-      <c r="D21" s="10"/>
+      <c r="D21" s="16"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="31"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="17"/>
       <c r="J21" s="31"/>
-      <c r="K21" s="21"/>
+      <c r="K21" s="31"/>
       <c r="L21" s="21"/>
       <c r="M21" s="21"/>
       <c r="N21" s="21"/>
@@ -1154,21 +1180,22 @@
       <c r="R21" s="21"/>
       <c r="S21" s="21"/>
       <c r="T21" s="21"/>
-      <c r="U21" s="12"/>
-      <c r="V21" s="18"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U21" s="21"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="18"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" s="16"/>
+      <c r="B22" s="2"/>
       <c r="C22" s="16"/>
-      <c r="D22" s="10"/>
+      <c r="D22" s="16"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="31"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="17"/>
       <c r="J22" s="31"/>
-      <c r="K22" s="21"/>
+      <c r="K22" s="31"/>
       <c r="L22" s="21"/>
       <c r="M22" s="21"/>
       <c r="N22" s="21"/>
@@ -1178,21 +1205,22 @@
       <c r="R22" s="21"/>
       <c r="S22" s="21"/>
       <c r="T22" s="21"/>
-      <c r="U22" s="12"/>
-      <c r="V22" s="18"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U22" s="21"/>
+      <c r="V22" s="12"/>
+      <c r="W22" s="18"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
-      <c r="B23" s="16"/>
+      <c r="B23" s="2"/>
       <c r="C23" s="16"/>
-      <c r="D23" s="10"/>
+      <c r="D23" s="16"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="31"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="17"/>
       <c r="J23" s="31"/>
-      <c r="K23" s="21"/>
+      <c r="K23" s="31"/>
       <c r="L23" s="21"/>
       <c r="M23" s="21"/>
       <c r="N23" s="21"/>
@@ -1202,21 +1230,22 @@
       <c r="R23" s="21"/>
       <c r="S23" s="21"/>
       <c r="T23" s="21"/>
-      <c r="U23" s="12"/>
-      <c r="V23" s="18"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U23" s="21"/>
+      <c r="V23" s="12"/>
+      <c r="W23" s="18"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="16"/>
+      <c r="B24" s="2"/>
       <c r="C24" s="16"/>
-      <c r="D24" s="10"/>
+      <c r="D24" s="16"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="31"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="17"/>
       <c r="J24" s="31"/>
-      <c r="K24" s="21"/>
+      <c r="K24" s="31"/>
       <c r="L24" s="21"/>
       <c r="M24" s="21"/>
       <c r="N24" s="21"/>
@@ -1226,21 +1255,22 @@
       <c r="R24" s="21"/>
       <c r="S24" s="21"/>
       <c r="T24" s="21"/>
-      <c r="U24" s="12"/>
-      <c r="V24" s="18"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U24" s="21"/>
+      <c r="V24" s="12"/>
+      <c r="W24" s="18"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" s="16"/>
+      <c r="B25" s="2"/>
       <c r="C25" s="16"/>
-      <c r="D25" s="10"/>
+      <c r="D25" s="16"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="31"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="17"/>
       <c r="J25" s="31"/>
-      <c r="K25" s="21"/>
+      <c r="K25" s="31"/>
       <c r="L25" s="21"/>
       <c r="M25" s="21"/>
       <c r="N25" s="21"/>
@@ -1250,21 +1280,22 @@
       <c r="R25" s="21"/>
       <c r="S25" s="21"/>
       <c r="T25" s="21"/>
-      <c r="U25" s="12"/>
-      <c r="V25" s="18"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U25" s="21"/>
+      <c r="V25" s="12"/>
+      <c r="W25" s="18"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="16"/>
+      <c r="B26" s="2"/>
       <c r="C26" s="16"/>
-      <c r="D26" s="10"/>
+      <c r="D26" s="16"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="31"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="17"/>
       <c r="J26" s="31"/>
-      <c r="K26" s="21"/>
+      <c r="K26" s="31"/>
       <c r="L26" s="21"/>
       <c r="M26" s="21"/>
       <c r="N26" s="21"/>
@@ -1274,21 +1305,22 @@
       <c r="R26" s="21"/>
       <c r="S26" s="21"/>
       <c r="T26" s="21"/>
-      <c r="U26" s="12"/>
-      <c r="V26" s="18"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U26" s="21"/>
+      <c r="V26" s="12"/>
+      <c r="W26" s="18"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="16"/>
+      <c r="B27" s="2"/>
       <c r="C27" s="16"/>
-      <c r="D27" s="10"/>
+      <c r="D27" s="16"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="31"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="17"/>
       <c r="J27" s="31"/>
-      <c r="K27" s="21"/>
+      <c r="K27" s="31"/>
       <c r="L27" s="21"/>
       <c r="M27" s="21"/>
       <c r="N27" s="21"/>
@@ -1298,21 +1330,22 @@
       <c r="R27" s="21"/>
       <c r="S27" s="21"/>
       <c r="T27" s="21"/>
-      <c r="U27" s="12"/>
-      <c r="V27" s="18"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="U27" s="21"/>
+      <c r="V27" s="12"/>
+      <c r="W27" s="18"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="16"/>
+      <c r="B28" s="2"/>
       <c r="C28" s="16"/>
-      <c r="D28" s="10"/>
+      <c r="D28" s="16"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="31"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="17"/>
       <c r="J28" s="31"/>
-      <c r="K28" s="21"/>
+      <c r="K28" s="31"/>
       <c r="L28" s="21"/>
       <c r="M28" s="21"/>
       <c r="N28" s="21"/>
@@ -1322,27 +1355,25 @@
       <c r="R28" s="21"/>
       <c r="S28" s="21"/>
       <c r="T28" s="21"/>
-      <c r="U28" s="12"/>
-      <c r="V28" s="18"/>
-    </row>
-    <row r="29" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U28" s="21"/>
+      <c r="V28" s="12"/>
+      <c r="W28" s="18"/>
+    </row>
+    <row r="29" spans="1:23" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="23"/>
       <c r="B29" s="24"/>
       <c r="C29" s="24"/>
       <c r="D29" s="24"/>
-      <c r="E29" s="25"/>
+      <c r="E29" s="24"/>
       <c r="F29" s="25"/>
       <c r="G29" s="25"/>
       <c r="H29" s="25"/>
-      <c r="I29" s="29">
-        <f xml:space="preserve"> SUM(I$5:I28)</f>
-        <v>0</v>
-      </c>
-      <c r="J29" s="29">
+      <c r="I29" s="25"/>
+      <c r="J29" s="32">
         <f xml:space="preserve"> SUM(J$5:J28)</f>
         <v>0</v>
       </c>
-      <c r="K29" s="29">
+      <c r="K29" s="32">
         <f xml:space="preserve"> SUM(K$5:K28)</f>
         <v>0</v>
       </c>
@@ -1382,12 +1413,16 @@
         <f xml:space="preserve"> SUM(T$5:T28)</f>
         <v>0</v>
       </c>
-      <c r="U29" s="26"/>
-      <c r="V29" s="27"/>
+      <c r="U29" s="29">
+        <f xml:space="preserve"> SUM(U$5:U28)</f>
+        <v>0</v>
+      </c>
+      <c r="V29" s="26"/>
+      <c r="W29" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A1:T1"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>
   <pageSetup scale="95" orientation="landscape" r:id="rId1"/>

</xml_diff>